<commit_message>
added class one deliverables
</commit_message>
<xml_diff>
--- a/Jamica/Deliverables Tracking.xlsx
+++ b/Jamica/Deliverables Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2680" yWindow="1400" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Professionalism" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Deliverables Tracking</t>
   </si>
@@ -31,12 +31,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Feature Block Diagram</t>
-  </si>
-  <si>
-    <t>Product Definition.txt</t>
-  </si>
-  <si>
     <t>Hardware Block Diagram</t>
   </si>
   <si>
@@ -134,6 +128,15 @@
   </si>
   <si>
     <t xml:space="preserve">Independent </t>
+  </si>
+  <si>
+    <t>Flow Diagram</t>
+  </si>
+  <si>
+    <t>Functionality Definition.txt</t>
+  </si>
+  <si>
+    <t>End of Day</t>
   </si>
 </sst>
 </file>
@@ -214,7 +217,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="227">
+  <cellStyleXfs count="231">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -442,8 +445,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -491,8 +498,9 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="227">
+  <cellStyles count="231">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -606,6 +614,8 @@
     <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -719,6 +729,8 @@
     <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1118,7 +1130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1132,17 +1144,17 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16">
       <c r="A1" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="9"/>
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="18">
       <c r="A2" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" s="3"/>
     </row>
@@ -1153,7 +1165,7 @@
     </row>
     <row r="4" spans="1:7" ht="16">
       <c r="A4" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="9"/>
       <c r="D4" s="3"/>
@@ -1163,37 +1175,37 @@
         <v>0</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="32">
       <c r="A6" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16">
       <c r="A7" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="32">
       <c r="A8" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1210,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1229,16 +1241,16 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16">
       <c r="A1" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:11" ht="18">
       <c r="A2" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="18">
@@ -1247,7 +1259,7 @@
     </row>
     <row r="4" spans="1:11" ht="16">
       <c r="A4" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="9"/>
     </row>
@@ -1256,63 +1268,83 @@
         <v>0</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J5"/>
       <c r="K5"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="D6"/>
+        <v>36</v>
+      </c>
+      <c r="B6" s="12">
+        <v>1</v>
+      </c>
+      <c r="C6" s="17">
+        <v>42877</v>
+      </c>
+      <c r="D6" s="17">
+        <v>42879</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="D7"/>
+        <v>37</v>
+      </c>
+      <c r="B7" s="12">
+        <v>1</v>
+      </c>
+      <c r="C7" s="17">
+        <v>42877</v>
+      </c>
+      <c r="D7" s="17">
+        <v>42879</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="13"/>
       <c r="D8"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" s="13"/>
       <c r="D9"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B10" s="13"/>
       <c r="D10"/>
@@ -1323,56 +1355,56 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="13"/>
       <c r="D12"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="12"/>
       <c r="D13"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14" s="13"/>
       <c r="D14"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B15" s="13"/>
       <c r="D15"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B16" s="13"/>
       <c r="D16"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B17" s="13"/>
       <c r="D17"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B18" s="13"/>
       <c r="D18"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" s="13"/>
       <c r="D19"/>
@@ -1384,42 +1416,42 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B21" s="12"/>
       <c r="D21"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B22" s="12"/>
       <c r="D22"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B23" s="12"/>
       <c r="D23"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B24" s="12"/>
       <c r="D24"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B25" s="12"/>
       <c r="D25"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B26" s="12"/>
       <c r="D26"/>
@@ -1430,21 +1462,21 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B28" s="12"/>
       <c r="D28"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B29" s="12"/>
       <c r="D29"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B30" s="12"/>
       <c r="D30"/>

</xml_diff>

<commit_message>
Product Definition feedback with block diagram start
</commit_message>
<xml_diff>
--- a/Jamica/Deliverables Tracking.xlsx
+++ b/Jamica/Deliverables Tracking.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3520" yWindow="0" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Professionalism" sheetId="2" r:id="rId1"/>
     <sheet name="Hardware Development Process" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>Deliverables Tracking</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Task enumeration for Product Definition</t>
   </si>
   <si>
-    <t>Estimate Architecture Task Hours</t>
-  </si>
-  <si>
     <t xml:space="preserve">Independent </t>
   </si>
   <si>
@@ -134,6 +131,15 @@
   </si>
   <si>
     <t>End of Day</t>
+  </si>
+  <si>
+    <t>Eagle Setup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read through Eagle Tutorials </t>
+  </si>
+  <si>
+    <t>2:00pm</t>
   </si>
 </sst>
 </file>
@@ -214,8 +220,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="237">
+  <cellStyleXfs count="243">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -503,7 +515,7 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="237">
+  <cellStyles count="243">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -622,6 +634,9 @@
     <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -740,6 +755,9 @@
     <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1229,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1259,7 +1277,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="18">
@@ -1302,7 +1320,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="12">
         <v>1</v>
@@ -1314,12 +1332,12 @@
         <v>42879</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="12">
         <v>1</v>
@@ -1331,7 +1349,7 @@
         <v>42879</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1348,7 +1366,7 @@
         <v>42887</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1365,7 +1383,7 @@
         <v>42887</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1382,7 +1400,7 @@
         <v>42887</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1391,137 +1409,163 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="13"/>
-      <c r="D12"/>
+        <v>38</v>
+      </c>
+      <c r="B12" s="12">
+        <v>3</v>
+      </c>
+      <c r="C12" s="17">
+        <v>42885</v>
+      </c>
+      <c r="D12" s="17">
+        <v>42891</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="12"/>
-      <c r="D13"/>
+        <v>37</v>
+      </c>
+      <c r="B13" s="12">
+        <v>3</v>
+      </c>
+      <c r="C13" s="17">
+        <v>42885</v>
+      </c>
+      <c r="D13" s="17">
+        <v>42891</v>
+      </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="13"/>
-      <c r="D14"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B15" s="13"/>
       <c r="D15"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="2" t="s">
-        <v>7</v>
+      <c r="A16" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B16" s="13"/>
       <c r="D16"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" s="13"/>
       <c r="D17"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B18" s="13"/>
       <c r="D18"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="6" t="s">
-        <v>21</v>
+      <c r="A19" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B19" s="13"/>
       <c r="D19"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="6"/>
+      <c r="A20" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="B20" s="13"/>
       <c r="D20"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="6"/>
+      <c r="B21" s="13"/>
+      <c r="D21"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="B21" s="12"/>
-      <c r="D21"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="B22" s="12"/>
       <c r="D22"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B23" s="12"/>
       <c r="D23"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" s="12"/>
       <c r="D24"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="12"/>
       <c r="D25"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="5" t="s">
-        <v>20</v>
+      <c r="A26" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="B26" s="12"/>
       <c r="D26"/>
     </row>
     <row r="27" spans="1:4">
+      <c r="A27" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="B27" s="12"/>
       <c r="D27"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="B28" s="12"/>
       <c r="D28"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="3" t="s">
-        <v>22</v>
+      <c r="A29" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B29" s="12"/>
       <c r="D29"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B30" s="12"/>
       <c r="D30"/>
     </row>
     <row r="31" spans="1:4">
+      <c r="A31" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="B31" s="12"/>
+      <c r="D31"/>
     </row>
     <row r="32" spans="1:4">
       <c r="B32" s="12"/>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Updated deliverables for Realization
We will use perf board for the next proto and do a full PCB in the
summer session
</commit_message>
<xml_diff>
--- a/Jamica/Deliverables Tracking.xlsx
+++ b/Jamica/Deliverables Tracking.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="0" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4740" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Professionalism" sheetId="2" r:id="rId1"/>
     <sheet name="Hardware Development Process" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t>Deliverables Tracking</t>
   </si>
@@ -140,6 +141,24 @@
   </si>
   <si>
     <t>2:00pm</t>
+  </si>
+  <si>
+    <t>Source Parts</t>
+  </si>
+  <si>
+    <t>Solder Perf Board Prototype</t>
+  </si>
+  <si>
+    <t>Code Hello World</t>
+  </si>
+  <si>
+    <t>Feasibility Study</t>
+  </si>
+  <si>
+    <t>Lab Tools list</t>
+  </si>
+  <si>
+    <t>Delayed to summer session</t>
   </si>
 </sst>
 </file>
@@ -150,7 +169,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -202,6 +221,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -220,7 +245,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="243">
+  <cellStyleXfs count="257">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -464,8 +489,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -514,8 +553,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="243">
+  <cellStyles count="257">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -637,6 +693,13 @@
     <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -758,6 +821,13 @@
     <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1247,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1408,164 +1478,254 @@
       <c r="D11"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="12">
-        <v>3</v>
+      <c r="A12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="13">
+        <v>4</v>
       </c>
       <c r="C12" s="17">
-        <v>42885</v>
+        <v>42894</v>
       </c>
       <c r="D12" s="17">
-        <v>42891</v>
+        <v>42905</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="12">
-        <v>3</v>
+      <c r="A13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="13">
+        <v>4</v>
       </c>
       <c r="C13" s="17">
-        <v>42885</v>
+        <v>42894</v>
       </c>
       <c r="D13" s="17">
-        <v>42891</v>
+        <v>42905</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="5"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
+      <c r="A14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="13">
+        <v>4</v>
+      </c>
+      <c r="C14" s="17">
+        <v>42894</v>
+      </c>
+      <c r="D14" s="17">
+        <v>42905</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="13"/>
-      <c r="D15"/>
+        <v>42</v>
+      </c>
+      <c r="B15" s="13">
+        <v>4</v>
+      </c>
+      <c r="C15" s="17">
+        <v>42894</v>
+      </c>
+      <c r="D15" s="17">
+        <v>42912</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="13"/>
-      <c r="D16"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="2" t="s">
-        <v>7</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B16" s="13">
+        <v>4</v>
+      </c>
+      <c r="C16" s="17">
+        <v>42914</v>
+      </c>
+      <c r="D16" s="17">
+        <v>42917</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="B17" s="13"/>
       <c r="D17"/>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:6" s="20" customFormat="1">
+      <c r="A18" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="23">
+        <v>3</v>
+      </c>
+      <c r="C18" s="24">
+        <v>42885</v>
+      </c>
+      <c r="D18" s="24">
+        <v>42891</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="20" customFormat="1">
+      <c r="A19" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="23">
+        <v>3</v>
+      </c>
+      <c r="C19" s="24">
+        <v>42885</v>
+      </c>
+      <c r="D19" s="24">
+        <v>42891</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="20" customFormat="1">
+      <c r="A20" s="18"/>
+      <c r="B20" s="19"/>
+    </row>
+    <row r="21" spans="1:6" s="20" customFormat="1">
+      <c r="A21" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="22"/>
+    </row>
+    <row r="22" spans="1:6" s="20" customFormat="1">
+      <c r="A22" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="22"/>
+    </row>
+    <row r="23" spans="1:6" s="20" customFormat="1">
+      <c r="A23" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="22"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="D18"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="2" t="s">
+      <c r="B24" s="13"/>
+      <c r="D24"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="D19"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="6" t="s">
+      <c r="B25" s="13"/>
+      <c r="D25"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="D20"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="6"/>
-      <c r="B21" s="13"/>
-      <c r="D21"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="6" t="s">
+      <c r="B26" s="13"/>
+      <c r="D26"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="6"/>
+      <c r="B27" s="13"/>
+      <c r="D27"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="D22"/>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="12"/>
-      <c r="D23"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="12"/>
-      <c r="D24"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="12"/>
-      <c r="D25"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="12"/>
-      <c r="D26"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="12"/>
-      <c r="D27"/>
-    </row>
-    <row r="28" spans="1:4">
       <c r="B28" s="12"/>
       <c r="D28"/>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="6" t="s">
-        <v>21</v>
+    <row r="29" spans="1:6">
+      <c r="A29" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="B29" s="12"/>
       <c r="D29"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:6">
       <c r="A30" s="3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B30" s="12"/>
       <c r="D30"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:6">
       <c r="A31" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B31" s="12"/>
       <c r="D31"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:6">
+      <c r="A32" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="B32" s="12"/>
-    </row>
-    <row r="33" spans="2:2">
+      <c r="D32"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="B33" s="12"/>
+      <c r="D33"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="B34" s="12"/>
+      <c r="D34"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="12"/>
+      <c r="D35"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="12"/>
+      <c r="D36"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="12"/>
+      <c r="D37"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="B38" s="12"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="B39" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1576,4 +1736,23 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Professionalism and HDP deliverables
</commit_message>
<xml_diff>
--- a/Jamica/Deliverables Tracking.xlsx
+++ b/Jamica/Deliverables Tracking.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Professionalism" sheetId="2" r:id="rId1"/>
     <sheet name="Hardware Development Process" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
   <si>
     <t>Deliverables Tracking</t>
   </si>
@@ -80,9 +80,6 @@
     <t xml:space="preserve">Session </t>
   </si>
   <si>
-    <t>ENTER DATE</t>
-  </si>
-  <si>
     <t>Estimate Task Hours</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>Review, Release, Version Control Lists</t>
   </si>
   <si>
-    <t xml:space="preserve">Derek Meng </t>
-  </si>
-  <si>
     <t>Estimated Hours</t>
   </si>
   <si>
@@ -119,9 +113,6 @@
     <t>Choose a task list format</t>
   </si>
   <si>
-    <t>Task enumeration for Product Definition</t>
-  </si>
-  <si>
     <t xml:space="preserve">Independent </t>
   </si>
   <si>
@@ -159,6 +150,24 @@
   </si>
   <si>
     <t>Delayed to summer session</t>
+  </si>
+  <si>
+    <t>Summer Session</t>
+  </si>
+  <si>
+    <t>GUI Implementation</t>
+  </si>
+  <si>
+    <t>RemotePi App Tested</t>
+  </si>
+  <si>
+    <t>Beginning of Class</t>
+  </si>
+  <si>
+    <t>6:00pm</t>
+  </si>
+  <si>
+    <t>Summer 2017</t>
   </si>
 </sst>
 </file>
@@ -169,7 +178,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -227,6 +236,11 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -245,7 +259,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="257">
+  <cellStyleXfs count="263">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -503,8 +517,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -570,8 +590,11 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="257">
+  <cellStyles count="263">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -700,6 +723,9 @@
     <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -828,6 +854,9 @@
     <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1225,10 +1254,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1239,46 +1268,46 @@
     <col min="7" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16">
+    <row r="1" spans="1:6" ht="16">
       <c r="A1" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="9"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="18">
+    <row r="2" spans="1:6" ht="18">
       <c r="A2" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="18">
+    <row r="3" spans="1:6" ht="18">
       <c r="A3" s="8"/>
       <c r="B3" s="10"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="16">
+    <row r="4" spans="1:6" ht="16">
       <c r="A4" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="9"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="30">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="30">
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>15</v>
@@ -1286,24 +1315,43 @@
       <c r="F5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="32">
-      <c r="A6" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="16">
-      <c r="A7" s="15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="32">
-      <c r="A8" s="15" t="s">
-        <v>32</v>
-      </c>
+    </row>
+    <row r="6" spans="1:6" ht="32">
+      <c r="A6" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="17">
+        <v>42921</v>
+      </c>
+      <c r="D6" s="17">
+        <v>42935</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16">
+      <c r="A7" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="17">
+        <v>42921</v>
+      </c>
+      <c r="D7" s="17">
+        <v>42935</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16">
+      <c r="A8" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1317,10 +1365,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1347,7 +1395,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="18">
@@ -1356,7 +1404,7 @@
     </row>
     <row r="4" spans="1:11" ht="16">
       <c r="A4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="9"/>
     </row>
@@ -1365,13 +1413,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>15</v>
@@ -1380,17 +1428,17 @@
         <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J5"/>
       <c r="K5"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6" s="12">
         <v>1</v>
@@ -1402,12 +1450,12 @@
         <v>42879</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B7" s="12">
         <v>1</v>
@@ -1419,7 +1467,7 @@
         <v>42879</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1436,7 +1484,7 @@
         <v>42887</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1453,7 +1501,7 @@
         <v>42887</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1470,7 +1518,7 @@
         <v>42887</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1479,7 +1527,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B12" s="13">
         <v>4</v>
@@ -1491,12 +1539,12 @@
         <v>42905</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B13" s="13">
         <v>4</v>
@@ -1508,12 +1556,12 @@
         <v>42905</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B14" s="13">
         <v>4</v>
@@ -1525,12 +1573,12 @@
         <v>42905</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B15" s="13">
         <v>4</v>
@@ -1542,12 +1590,12 @@
         <v>42912</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B16" s="13">
         <v>4</v>
@@ -1559,173 +1607,220 @@
         <v>42917</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="B17" s="13"/>
-      <c r="D17"/>
-    </row>
-    <row r="18" spans="1:6" s="20" customFormat="1">
-      <c r="A18" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="23">
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="13">
+        <v>1</v>
+      </c>
+      <c r="C19" s="17">
+        <v>42921</v>
+      </c>
+      <c r="D19" s="17">
+        <v>42924</v>
+      </c>
+      <c r="E19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="13">
+        <v>1</v>
+      </c>
+      <c r="C20" s="17">
+        <v>42921</v>
+      </c>
+      <c r="D20" s="17">
+        <v>42924</v>
+      </c>
+      <c r="E20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="B21" s="13"/>
+      <c r="D21"/>
+    </row>
+    <row r="22" spans="1:6" s="20" customFormat="1">
+      <c r="A22" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="23">
         <v>3</v>
       </c>
-      <c r="C18" s="24">
+      <c r="C22" s="24">
         <v>42885</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D22" s="24">
         <v>42891</v>
       </c>
-      <c r="E18" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="20" customFormat="1">
-      <c r="A19" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="23">
-        <v>3</v>
-      </c>
-      <c r="C19" s="24">
-        <v>42885</v>
-      </c>
-      <c r="D19" s="24">
-        <v>42891</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="20" customFormat="1">
-      <c r="A20" s="18"/>
-      <c r="B20" s="19"/>
-    </row>
-    <row r="21" spans="1:6" s="20" customFormat="1">
-      <c r="A21" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="22"/>
-    </row>
-    <row r="22" spans="1:6" s="20" customFormat="1">
-      <c r="A22" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="22"/>
+      <c r="E22" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="23" spans="1:6" s="20" customFormat="1">
       <c r="A23" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="23">
+        <v>3</v>
+      </c>
+      <c r="C23" s="24">
+        <v>42885</v>
+      </c>
+      <c r="D23" s="24">
+        <v>42891</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="20" customFormat="1">
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
+    </row>
+    <row r="25" spans="1:6" s="20" customFormat="1">
+      <c r="A25" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="22"/>
+    </row>
+    <row r="26" spans="1:6" s="20" customFormat="1">
+      <c r="A26" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="22"/>
+    </row>
+    <row r="27" spans="1:6" s="20" customFormat="1">
+      <c r="A27" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="22"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="2" t="s">
+      <c r="B27" s="22"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="D24"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="2" t="s">
+      <c r="B28" s="13"/>
+      <c r="D28"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="D25"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="13"/>
-      <c r="D26"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="6"/>
-      <c r="B27" s="13"/>
-      <c r="D27"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="12"/>
-      <c r="D28"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="12"/>
+      <c r="B29" s="13"/>
       <c r="D29"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="12"/>
+      <c r="A30" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="13"/>
       <c r="D30"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="12"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="13"/>
       <c r="D31"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="3" t="s">
-        <v>13</v>
+      <c r="A32" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="B32" s="12"/>
       <c r="D32"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="5" t="s">
-        <v>20</v>
+      <c r="A33" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="B33" s="12"/>
       <c r="D33"/>
     </row>
     <row r="34" spans="1:4">
+      <c r="A34" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="B34" s="12"/>
       <c r="D34"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="6" t="s">
-        <v>21</v>
+      <c r="A35" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B35" s="12"/>
       <c r="D35"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B36" s="12"/>
       <c r="D36"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="3" t="s">
-        <v>16</v>
+      <c r="A37" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="B37" s="12"/>
       <c r="D37"/>
     </row>
     <row r="38" spans="1:4">
       <c r="B38" s="12"/>
+      <c r="D38"/>
     </row>
     <row r="39" spans="1:4">
+      <c r="A39" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="B39" s="12"/>
+      <c r="D39"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="12"/>
+      <c r="D40"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="12"/>
+      <c r="D41"/>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="B42" s="12"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="B43" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
updated deliverables and task enumeration
</commit_message>
<xml_diff>
--- a/Jamica/Deliverables Tracking.xlsx
+++ b/Jamica/Deliverables Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-35900" yWindow="200" windowWidth="26200" windowHeight="18500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Professionalism" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
   <si>
     <t>Deliverables Tracking</t>
   </si>
@@ -168,6 +168,15 @@
   </si>
   <si>
     <t>Summer 2017</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extend GUI </t>
+  </si>
+  <si>
+    <t>Sewing the Hat</t>
   </si>
 </sst>
 </file>
@@ -259,8 +268,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="263">
+  <cellStyleXfs count="269">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -594,7 +609,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="263">
+  <cellStyles count="269">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -726,6 +741,9 @@
     <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -857,6 +875,9 @@
     <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1257,7 +1278,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A6" sqref="A6:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1365,10 +1386,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1378,19 +1399,20 @@
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16">
+    <row r="1" spans="1:12" ht="16">
       <c r="A1" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:11" ht="18">
+    <row r="2" spans="1:12" ht="18">
       <c r="A2" s="8" t="s">
         <v>18</v>
       </c>
@@ -1398,17 +1420,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="18">
+    <row r="3" spans="1:12" ht="18">
       <c r="A3" s="8"/>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:11" ht="16">
+    <row r="4" spans="1:12" ht="16">
       <c r="A4" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="9"/>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="30">
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="30">
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
@@ -1424,19 +1446,22 @@
       <c r="E5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J5"/>
       <c r="K5"/>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
@@ -1453,7 +1478,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
         <v>32</v>
       </c>
@@ -1470,7 +1495,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1487,7 +1512,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1504,7 +1529,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -1521,11 +1546,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:12">
       <c r="B11" s="13"/>
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
@@ -1542,7 +1567,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12">
       <c r="A13" s="3" t="s">
         <v>41</v>
       </c>
@@ -1559,7 +1584,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12">
       <c r="A14" s="3" t="s">
         <v>40</v>
       </c>
@@ -1576,7 +1601,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12">
       <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
@@ -1593,7 +1618,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:12">
       <c r="A16" s="3" t="s">
         <v>38</v>
       </c>
@@ -1609,13 +1634,16 @@
       <c r="E16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="F16" s="17">
+        <v>42926</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="B17" s="13"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7">
       <c r="A18" s="4" t="s">
         <v>43</v>
       </c>
@@ -1623,7 +1651,7 @@
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:7">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
@@ -1640,7 +1668,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7">
       <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
@@ -1657,142 +1685,157 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="B21" s="13"/>
-      <c r="D21"/>
-    </row>
-    <row r="22" spans="1:6" s="20" customFormat="1">
-      <c r="A22" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="23">
-        <v>3</v>
-      </c>
-      <c r="C22" s="24">
-        <v>42885</v>
-      </c>
-      <c r="D22" s="24">
-        <v>42891</v>
-      </c>
-      <c r="E22" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="20" customFormat="1">
-      <c r="A23" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="23">
-        <v>3</v>
-      </c>
-      <c r="C23" s="24">
-        <v>42885</v>
-      </c>
-      <c r="D23" s="24">
-        <v>42891</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="20" customFormat="1">
-      <c r="A24" s="18"/>
-      <c r="B24" s="19"/>
-    </row>
-    <row r="25" spans="1:6" s="20" customFormat="1">
-      <c r="A25" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="22"/>
-    </row>
-    <row r="26" spans="1:6" s="20" customFormat="1">
-      <c r="A26" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="22"/>
-    </row>
-    <row r="27" spans="1:6" s="20" customFormat="1">
-      <c r="A27" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="22"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="2" t="s">
-        <v>8</v>
-      </c>
+    <row r="21" spans="1:7">
+      <c r="A21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="13">
+        <v>2</v>
+      </c>
+      <c r="C21" s="17">
+        <v>42924</v>
+      </c>
+      <c r="D21" s="17">
+        <v>42926</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="13">
+        <v>2</v>
+      </c>
+      <c r="C22" s="17">
+        <v>42924</v>
+      </c>
+      <c r="D22" s="17">
+        <v>42926</v>
+      </c>
+      <c r="E22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="B23" s="13"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="B24" s="13"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="B25" s="13"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="B26" s="13"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="B27" s="13"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+    </row>
+    <row r="28" spans="1:7">
       <c r="B28" s="13"/>
       <c r="D28"/>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:7" s="20" customFormat="1">
+      <c r="A29" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="23">
+        <v>3</v>
+      </c>
+      <c r="C29" s="24">
+        <v>42885</v>
+      </c>
+      <c r="D29" s="24">
+        <v>42891</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="24"/>
+      <c r="G29" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="20" customFormat="1">
+      <c r="A30" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="23">
+        <v>3</v>
+      </c>
+      <c r="C30" s="24">
+        <v>42885</v>
+      </c>
+      <c r="D30" s="24">
+        <v>42891</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="24"/>
+      <c r="G30" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="20" customFormat="1">
+      <c r="A31" s="18"/>
+      <c r="B31" s="19"/>
+    </row>
+    <row r="32" spans="1:7" s="20" customFormat="1">
+      <c r="A32" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="22"/>
+    </row>
+    <row r="33" spans="1:4" s="20" customFormat="1">
+      <c r="A33" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="22"/>
+    </row>
+    <row r="34" spans="1:4" s="20" customFormat="1">
+      <c r="A34" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="22"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="D35"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="D29"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="6" t="s">
+      <c r="B36" s="13"/>
+      <c r="D36"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="D30"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="6"/>
-      <c r="B31" s="13"/>
-      <c r="D31"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="12"/>
-      <c r="D32"/>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="12"/>
-      <c r="D33"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B34" s="12"/>
-      <c r="D34"/>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="12"/>
-      <c r="D35"/>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="12"/>
-      <c r="D36"/>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B37" s="12"/>
+      <c r="B37" s="13"/>
       <c r="D37"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="B38" s="12"/>
+      <c r="A38" s="6"/>
+      <c r="B38" s="13"/>
       <c r="D38"/>
     </row>
     <row r="39" spans="1:4">
@@ -1804,23 +1847,69 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B40" s="12"/>
       <c r="D40"/>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B41" s="12"/>
       <c r="D41"/>
     </row>
     <row r="42" spans="1:4">
+      <c r="A42" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="B42" s="12"/>
+      <c r="D42"/>
     </row>
     <row r="43" spans="1:4">
+      <c r="A43" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="B43" s="12"/>
+      <c r="D43"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="12"/>
+      <c r="D44"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="B45" s="12"/>
+      <c r="D45"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" s="12"/>
+      <c r="D46"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" s="12"/>
+      <c r="D47"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="12"/>
+      <c r="D48"/>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="12"/>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>